<commit_message>
feat: atualiza orcamento 2026 para versao BUD_V2 conforme planilha
</commit_message>
<xml_diff>
--- a/orçamento.xlsx
+++ b/orçamento.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brqbnwvfs02vs\Departamentos\PA\_SGVM_\LCP\GESTÃO\TRATAMENTO DE ANOMALIA\2026\Indicadores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40000398\OneDrive - ArcelorMittal\Desktop\n8n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3E41674-D437-4828-8D1E-12027EAC1562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81AFD91-B690-4BAB-ACA4-78DA3501777C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TL1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,8 @@
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="47">
   <si>
     <t>Produção (t)</t>
   </si>
@@ -184,15 +186,19 @@
   <si>
     <t>Índice de Qualidade %</t>
   </si>
+  <si>
+    <t>vp</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -341,7 +347,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,6 +402,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="27">
     <border>
@@ -768,7 +780,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -982,6 +994,26 @@
     <xf numFmtId="10" fontId="13" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="6" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="11" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="6" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1164,76 +1196,6 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
-      <sheetName val="TL1"/>
-      <sheetName val="TL2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1">
-        <row r="4">
-          <cell r="N4">
-            <v>267672.11300000001</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="N5">
-            <v>96.337613040616304</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="N6">
-            <v>71.458289083355865</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="N7">
-            <v>40.240817019764272</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="N8">
-            <v>-34.532430279868798</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1">
-        <row r="4">
-          <cell r="N4">
-            <v>15010</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="N5">
-            <v>93.670886075949369</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="N6">
-            <v>100.00639819453697</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="N7">
-            <v>72.418387741505668</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="N8">
-            <v>-62.328447701532312</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
       <sheetName val="Produções"/>
       <sheetName val="Rateio SF"/>
       <sheetName val="Rateio SF (2)"/>
@@ -1285,6 +1247,173 @@
       <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3" refreshError="1"/>
       <sheetData sheetId="4" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="TL1"/>
+      <sheetName val="TL2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1">
+        <row r="4">
+          <cell r="N4">
+            <v>15010</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="N5">
+            <v>93.670886075949369</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="N6">
+            <v>100.00639819453697</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="N7">
+            <v>72.418387741505668</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="N8">
+            <v>-62.328447701532312</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Produção 2026"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="36">
+          <cell r="E36">
+            <v>9500.384</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="F37">
+            <v>30216</v>
+          </cell>
+          <cell r="G37">
+            <v>34705</v>
+          </cell>
+          <cell r="H37">
+            <v>32442</v>
+          </cell>
+          <cell r="I37">
+            <v>33304.999999999003</v>
+          </cell>
+          <cell r="J37">
+            <v>28737.000000000997</v>
+          </cell>
+          <cell r="K37">
+            <v>29542</v>
+          </cell>
+          <cell r="L37">
+            <v>40642</v>
+          </cell>
+          <cell r="M37">
+            <v>45937</v>
+          </cell>
+          <cell r="N37">
+            <v>46978</v>
+          </cell>
+          <cell r="O37">
+            <v>45432</v>
+          </cell>
+          <cell r="P37">
+            <v>35164</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="TL1"/>
+      <sheetName val="Planilha1"/>
+      <sheetName val="TL2"/>
+      <sheetName val="TL1+TL2"/>
+      <sheetName val="Comparação Médio"/>
+      <sheetName val="Resumo Produção"/>
+      <sheetName val="KPIs Real"/>
+      <sheetName val="Dados e-mail"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2">
+        <row r="4">
+          <cell r="C4">
+            <v>9816</v>
+          </cell>
+          <cell r="D4">
+            <v>11705</v>
+          </cell>
+          <cell r="E4">
+            <v>10642</v>
+          </cell>
+          <cell r="F4">
+            <v>11005</v>
+          </cell>
+          <cell r="G4">
+            <v>17537</v>
+          </cell>
+          <cell r="H4">
+            <v>18142</v>
+          </cell>
+          <cell r="I4">
+            <v>18142</v>
+          </cell>
+          <cell r="J4">
+            <v>24437</v>
+          </cell>
+          <cell r="K4">
+            <v>24978</v>
+          </cell>
+          <cell r="L4">
+            <v>24132</v>
+          </cell>
+          <cell r="M4">
+            <v>13164</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1596,26 +1725,26 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:N8"/>
+      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="8.1796875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.1796875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="0.81640625" customWidth="1"/>
-    <col min="16" max="16" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="0.453125" customWidth="1"/>
-    <col min="18" max="18" width="11.1796875" customWidth="1"/>
-    <col min="19" max="19" width="0.81640625" customWidth="1"/>
-    <col min="20" max="20" width="60.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="8.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="0.85546875" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="0.42578125" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" customWidth="1"/>
+    <col min="19" max="19" width="0.85546875" customWidth="1"/>
+    <col min="20" max="20" width="60.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="53"/>
       <c r="N1" s="22">
         <f>'[1]Produção 2026'!$R$35</f>
@@ -1623,15 +1752,15 @@
       </c>
       <c r="O1" s="22">
         <f>N4+'TL2'!N4</f>
-        <v>429200</v>
+        <v>427818.27</v>
       </c>
       <c r="Q1" s="22">
         <f>N1-O1</f>
-        <v>0</v>
+        <v>1381.7299999999814</v>
       </c>
       <c r="S1" s="22"/>
     </row>
-    <row r="2" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="79" t="s">
         <v>32</v>
       </c>
@@ -1675,7 +1804,7 @@
         <v>33</v>
       </c>
       <c r="P2" s="39" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="R2" s="75" t="s">
         <v>34</v>
@@ -1684,7 +1813,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="79"/>
       <c r="B3" s="28" t="s">
         <v>5</v>
@@ -1731,291 +1860,285 @@
       <c r="R3" s="76"/>
       <c r="T3" s="78"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="26">
-        <f>'[1]Produção 2026'!E35-'TL2'!B4</f>
+      <c r="B4" s="87">
+        <v>17118.27</v>
+      </c>
+      <c r="C4" s="26">
+        <f>'[4]Produção 2026'!F37-[5]TL2!C4</f>
+        <v>20400</v>
+      </c>
+      <c r="D4" s="26">
+        <f>'[4]Produção 2026'!G37-[5]TL2!D4</f>
+        <v>23000</v>
+      </c>
+      <c r="E4" s="26">
+        <f>'[4]Produção 2026'!H37-[5]TL2!E4</f>
+        <v>21800</v>
+      </c>
+      <c r="F4" s="26">
+        <f>'[4]Produção 2026'!I37-[5]TL2!F4</f>
+        <v>22299.999999999003</v>
+      </c>
+      <c r="G4" s="26">
+        <f>'[4]Produção 2026'!J37-[5]TL2!G4</f>
+        <v>11200.000000000997</v>
+      </c>
+      <c r="H4" s="26">
+        <f>'[4]Produção 2026'!K37-[5]TL2!H4</f>
+        <v>11400</v>
+      </c>
+      <c r="I4" s="26">
+        <f>'[4]Produção 2026'!L37-[5]TL2!I4</f>
+        <v>22500</v>
+      </c>
+      <c r="J4" s="26">
+        <f>'[4]Produção 2026'!M37-[5]TL2!J4</f>
+        <v>21500</v>
+      </c>
+      <c r="K4" s="26">
+        <f>'[4]Produção 2026'!N37-[5]TL2!K4</f>
         <v>22000</v>
       </c>
-      <c r="C4" s="26">
-        <f>'[1]Produção 2026'!F35-'TL2'!C4</f>
-        <v>19900</v>
-      </c>
-      <c r="D4" s="26">
-        <f>'[1]Produção 2026'!G35-'TL2'!D4</f>
-        <v>22000</v>
-      </c>
-      <c r="E4" s="26">
-        <f>'[1]Produção 2026'!H35-'TL2'!E4</f>
+      <c r="L4" s="26">
+        <f>'[4]Produção 2026'!O37-[5]TL2!L4</f>
         <v>21300</v>
       </c>
-      <c r="F4" s="26">
-        <f>'[1]Produção 2026'!I35-'TL2'!F4</f>
-        <v>22000</v>
-      </c>
-      <c r="G4" s="26">
-        <f>'[1]Produção 2026'!J35-'TL2'!G4</f>
-        <v>10700</v>
-      </c>
-      <c r="H4" s="26">
-        <f>'[1]Produção 2026'!K35-'TL2'!H4</f>
-        <v>11400</v>
-      </c>
-      <c r="I4" s="26">
-        <f>'[1]Produção 2026'!L35-'TL2'!I4</f>
-        <v>22000</v>
-      </c>
-      <c r="J4" s="26">
-        <f>'[1]Produção 2026'!M35-'TL2'!J4</f>
-        <v>21300</v>
-      </c>
-      <c r="K4" s="26">
-        <f>'[1]Produção 2026'!N35-'TL2'!K4</f>
-        <v>22000</v>
-      </c>
-      <c r="L4" s="26">
-        <f>'[1]Produção 2026'!O35-'TL2'!L4</f>
-        <v>21300</v>
-      </c>
       <c r="M4" s="26">
-        <f>'[1]Produção 2026'!P35-'TL2'!M4</f>
+        <f>'[4]Produção 2026'!P37-[5]TL2!M4</f>
         <v>22000</v>
       </c>
       <c r="N4" s="49">
         <f>SUM(B4:M4)</f>
+        <v>236518.27</v>
+      </c>
+      <c r="P4" s="42">
         <v>237900</v>
-      </c>
-      <c r="P4" s="42">
-        <f>[2]TL1!$N4</f>
-        <v>267672.11300000001</v>
       </c>
       <c r="R4" s="36">
         <f>N4-P4</f>
-        <v>-29772.113000000012</v>
+        <v>-1381.7300000000105</v>
       </c>
       <c r="T4" s="29"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="88">
+        <v>96.314533390790302</v>
+      </c>
+      <c r="C5" s="89">
         <v>96.3</v>
       </c>
-      <c r="C5" s="23">
-        <v>96.3</v>
-      </c>
-      <c r="D5" s="23">
-        <v>96.32</v>
-      </c>
-      <c r="E5" s="23">
+      <c r="D5" s="89">
         <v>96.34</v>
       </c>
-      <c r="F5" s="23">
+      <c r="E5" s="89">
         <v>96.34</v>
       </c>
-      <c r="G5" s="23">
+      <c r="F5" s="89">
         <v>96.34</v>
       </c>
-      <c r="H5" s="23">
+      <c r="G5" s="89">
         <v>96.34</v>
       </c>
-      <c r="I5" s="23">
+      <c r="H5" s="89">
         <v>96.34</v>
       </c>
-      <c r="J5" s="23">
+      <c r="I5" s="89">
         <v>96.34</v>
       </c>
-      <c r="K5" s="23">
+      <c r="J5" s="89">
         <v>96.34</v>
       </c>
-      <c r="L5" s="23">
-        <v>96.37</v>
-      </c>
-      <c r="M5" s="23">
-        <v>96.37</v>
+      <c r="K5" s="89">
+        <v>96.41</v>
+      </c>
+      <c r="L5" s="89">
+        <v>96.42</v>
+      </c>
+      <c r="M5" s="89">
+        <v>96.42</v>
       </c>
       <c r="N5" s="50">
         <f>SUMPRODUCT($B$4:$M$4,B5:M5)/$N$4</f>
-        <v>96.336565783942831</v>
+        <v>96.355863703499807</v>
       </c>
       <c r="P5" s="41">
-        <f>[2]TL1!$N5</f>
-        <v>96.337613040616304</v>
+        <v>96.360000000000014</v>
       </c>
       <c r="R5" s="36">
         <f>N5-P5</f>
-        <v>-1.0472566734733846E-3</v>
+        <v>-4.1362965002065266E-3</v>
       </c>
       <c r="T5" s="80" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="23">
-        <v>74.8</v>
-      </c>
-      <c r="C6" s="23">
-        <v>76</v>
-      </c>
-      <c r="D6" s="23">
-        <v>74.8</v>
-      </c>
-      <c r="E6" s="23">
-        <v>74.900000000000006</v>
-      </c>
-      <c r="F6" s="23">
-        <v>74.8</v>
-      </c>
-      <c r="G6" s="23">
-        <v>76</v>
-      </c>
-      <c r="H6" s="23">
-        <v>81</v>
-      </c>
-      <c r="I6" s="23">
-        <v>74.8</v>
-      </c>
-      <c r="J6" s="23">
-        <v>74.900000000000006</v>
-      </c>
-      <c r="K6" s="23">
-        <v>74.8</v>
-      </c>
-      <c r="L6" s="23">
-        <v>74.900000000000006</v>
-      </c>
-      <c r="M6" s="23">
-        <v>74.8</v>
+      <c r="B6" s="88">
+        <v>80.762133089380001</v>
+      </c>
+      <c r="C6" s="89">
+        <v>75</v>
+      </c>
+      <c r="D6" s="89">
+        <v>75</v>
+      </c>
+      <c r="E6" s="89">
+        <v>75</v>
+      </c>
+      <c r="F6" s="89">
+        <v>75</v>
+      </c>
+      <c r="G6" s="89">
+        <v>75</v>
+      </c>
+      <c r="H6" s="89">
+        <v>75</v>
+      </c>
+      <c r="I6" s="90">
+        <v>75</v>
+      </c>
+      <c r="J6" s="89">
+        <v>75</v>
+      </c>
+      <c r="K6" s="89">
+        <v>75</v>
+      </c>
+      <c r="L6" s="89">
+        <v>73</v>
+      </c>
+      <c r="M6" s="89">
+        <v>72</v>
       </c>
       <c r="N6" s="50">
         <f>SUMPRODUCT($B$4:$M$4,B6:M6)/$N$4</f>
-        <v>75.278310214375793</v>
+        <v>74.957879575222421</v>
       </c>
       <c r="P6" s="41">
-        <f>[2]TL1!$N6</f>
-        <v>71.458289083355865</v>
+        <v>75</v>
       </c>
       <c r="R6" s="36">
         <f>N6-P6</f>
-        <v>3.8200211310199279</v>
+        <v>-4.2120424777579046E-2</v>
       </c>
       <c r="T6" s="81"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="23">
-        <v>42</v>
-      </c>
-      <c r="C7" s="23">
-        <v>42.5</v>
-      </c>
-      <c r="D7" s="23">
-        <v>42</v>
-      </c>
-      <c r="E7" s="23">
-        <v>42.5</v>
-      </c>
-      <c r="F7" s="23">
-        <v>42</v>
-      </c>
-      <c r="G7" s="23">
-        <v>42</v>
-      </c>
-      <c r="H7" s="23">
-        <v>45</v>
-      </c>
-      <c r="I7" s="23">
-        <v>41.2</v>
-      </c>
-      <c r="J7" s="23">
-        <v>41.2</v>
-      </c>
-      <c r="K7" s="23">
-        <v>41.2</v>
-      </c>
-      <c r="L7" s="23">
-        <v>41.2</v>
-      </c>
-      <c r="M7" s="23">
-        <v>41.2</v>
-      </c>
-      <c r="N7" s="50">
+      <c r="B7" s="88">
+        <v>45.395826542185716</v>
+      </c>
+      <c r="C7" s="89">
+        <v>41.95</v>
+      </c>
+      <c r="D7" s="89">
+        <v>41.83</v>
+      </c>
+      <c r="E7" s="89">
+        <v>42.08</v>
+      </c>
+      <c r="F7" s="89">
+        <v>41.83</v>
+      </c>
+      <c r="G7" s="89">
+        <v>41.5</v>
+      </c>
+      <c r="H7" s="89">
+        <v>42.43</v>
+      </c>
+      <c r="I7" s="90">
+        <v>41</v>
+      </c>
+      <c r="J7" s="89">
+        <v>40</v>
+      </c>
+      <c r="K7" s="89">
+        <v>39</v>
+      </c>
+      <c r="L7" s="89">
+        <v>38</v>
+      </c>
+      <c r="M7" s="89">
+        <v>38</v>
+      </c>
+      <c r="N7" s="91">
         <f>SUMPRODUCT($B$4:$M$4,B7:M7)/$N$4</f>
-        <v>41.865153425809162</v>
+        <v>40.925054185548973</v>
       </c>
       <c r="P7" s="41">
-        <f>[2]TL1!$N7</f>
-        <v>40.240817019764272</v>
+        <v>41</v>
       </c>
       <c r="R7" s="36">
         <f>N7-P7</f>
-        <v>1.6243364060448897</v>
+        <v>-7.4945814451027104E-2</v>
       </c>
       <c r="T7" s="82"/>
     </row>
-    <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="27">
-        <v>-34.200000000000003</v>
-      </c>
-      <c r="C8" s="27">
-        <v>-34.4</v>
-      </c>
-      <c r="D8" s="27">
-        <v>-34.200000000000003</v>
-      </c>
-      <c r="E8" s="27">
-        <v>-34.4</v>
-      </c>
-      <c r="F8" s="27">
-        <v>-34.299999999999997</v>
-      </c>
-      <c r="G8" s="27">
-        <v>-35.700000000000003</v>
-      </c>
-      <c r="H8" s="27">
-        <v>-34.4</v>
-      </c>
-      <c r="I8" s="27">
-        <v>-34.4</v>
-      </c>
-      <c r="J8" s="27">
-        <v>-34.4</v>
-      </c>
-      <c r="K8" s="27">
-        <v>-34.4</v>
-      </c>
-      <c r="L8" s="27">
-        <v>-34.4</v>
-      </c>
-      <c r="M8" s="27">
-        <v>-35.700000000000003</v>
-      </c>
-      <c r="N8" s="51">
+      <c r="B8" s="92">
+        <v>-35.944636928850002</v>
+      </c>
+      <c r="C8" s="93">
+        <v>-34.53</v>
+      </c>
+      <c r="D8" s="93">
+        <v>-34</v>
+      </c>
+      <c r="E8" s="93">
+        <v>-34.53</v>
+      </c>
+      <c r="F8" s="93">
+        <v>-34.53</v>
+      </c>
+      <c r="G8" s="93">
+        <v>-34.53</v>
+      </c>
+      <c r="H8" s="93">
+        <v>-34.53</v>
+      </c>
+      <c r="I8" s="93">
+        <v>-34.53</v>
+      </c>
+      <c r="J8" s="93">
+        <v>-34.53</v>
+      </c>
+      <c r="K8" s="93">
+        <v>-34.53</v>
+      </c>
+      <c r="L8" s="93">
+        <v>-34.53</v>
+      </c>
+      <c r="M8" s="93">
+        <v>-34.53</v>
+      </c>
+      <c r="N8" s="94">
         <f>SUMPRODUCT($B$4:$M$4,B8:M8)/$N$4</f>
-        <v>-34.53245060949979</v>
+        <v>-34.580846545173976</v>
       </c>
       <c r="P8" s="41">
-        <f>[2]TL1!$N8</f>
-        <v>-34.532430279868798</v>
+        <v>-34.53</v>
       </c>
       <c r="R8" s="36">
         <f>N8-P8</f>
-        <v>-2.0329630991966496E-5</v>
+        <v>-5.0846545173975244E-2</v>
       </c>
       <c r="T8" s="29"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="59"/>
       <c r="B9" s="59"/>
       <c r="C9" s="60"/>
@@ -2036,30 +2159,30 @@
       <c r="R9" s="60"/>
       <c r="S9" s="60"/>
     </row>
-    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <f>B4/B5%</f>
-        <v>22845.27518172378</v>
+        <v>17773.299000000003</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ref="C10:N10" si="0">C4/C5%</f>
-        <v>20664.58982346833</v>
+        <v>21183.800623052961</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="0"/>
-        <v>22840.531561461794</v>
+        <v>23873.780361220677</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>22109.19659539132</v>
+        <v>22628.191820635249</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
-        <v>22835.789910732819</v>
+        <v>23147.187045878141</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>11106.497820220053</v>
+        <v>11625.493045465017</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="0"/>
@@ -2067,224 +2190,224 @@
       </c>
       <c r="I10" s="3">
         <f t="shared" si="0"/>
-        <v>22835.789910732819</v>
+        <v>23354.785135976748</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="0"/>
-        <v>22109.19659539132</v>
+        <v>22316.794685488894</v>
       </c>
       <c r="K10" s="3">
         <f t="shared" si="0"/>
-        <v>22835.789910732819</v>
+        <v>22819.209625557516</v>
       </c>
       <c r="L10" s="3">
         <f t="shared" si="0"/>
-        <v>22102.313998132198</v>
+        <v>22090.85252022402</v>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="0"/>
-        <v>22828.681124831379</v>
+        <v>22816.842978635137</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="0"/>
-        <v>246946.73104036751</v>
+        <v>245463.28672617071</v>
       </c>
       <c r="O10" s="3">
         <f>P4/P5%</f>
-        <v>277847.98123153462</v>
+        <v>246886.67496886672</v>
       </c>
       <c r="Q10" s="3"/>
       <c r="S10" s="3"/>
     </row>
-    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B8*B4/1000</f>
-        <v>-752.40000000000009</v>
+        <v>-615.31000000002518</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ref="C11:N11" si="1">C8*C4/1000</f>
-        <v>-684.56</v>
+        <v>-704.41200000000003</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="1"/>
-        <v>-752.40000000000009</v>
+        <v>-782</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="1"/>
-        <v>-732.72</v>
+        <v>-752.75400000000002</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="1"/>
-        <v>-754.59999999999991</v>
+        <v>-770.01899999996567</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" si="1"/>
-        <v>-381.99000000000007</v>
+        <v>-386.73600000003444</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="1"/>
-        <v>-392.16</v>
+        <v>-393.642</v>
       </c>
       <c r="I11" s="3">
         <f t="shared" si="1"/>
-        <v>-756.8</v>
+        <v>-776.92499999999995</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" si="1"/>
-        <v>-732.72</v>
+        <v>-742.39499999999998</v>
       </c>
       <c r="K11" s="3">
         <f t="shared" si="1"/>
-        <v>-756.8</v>
+        <v>-759.66</v>
       </c>
       <c r="L11" s="3">
         <f t="shared" si="1"/>
-        <v>-732.72</v>
+        <v>-735.48900000000003</v>
       </c>
       <c r="M11" s="3">
         <f t="shared" si="1"/>
-        <v>-785.40000000000009</v>
+        <v>-759.66</v>
       </c>
       <c r="N11" s="3">
         <f t="shared" si="1"/>
-        <v>-8215.27</v>
+        <v>-8179.002000000025</v>
       </c>
       <c r="O11" s="3">
         <f>P8*P4/1000</f>
-        <v>-9243.3685800376625</v>
+        <v>-8214.6869999999999</v>
       </c>
       <c r="Q11" s="3"/>
       <c r="S11" s="3"/>
     </row>
-    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f>B10-B4+B11</f>
-        <v>92.875181723780315</v>
+        <v>39.718999999977086</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:N12" si="2">C10-C4+C11</f>
-        <v>80.029823468330051</v>
+        <v>79.388623052960838</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="2"/>
-        <v>88.131561461793808</v>
+        <v>91.78036122067715</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="2"/>
-        <v>76.476595391320416</v>
+        <v>75.437820635249295</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="2"/>
-        <v>81.189910732819499</v>
+        <v>77.168045879172496</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="2"/>
-        <v>24.507820220052679</v>
+        <v>38.757045463985378</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" si="2"/>
-        <v>40.931135561551685</v>
+        <v>39.449135561551714</v>
       </c>
       <c r="I12" s="3">
         <f t="shared" si="2"/>
-        <v>78.989910732819453</v>
+        <v>77.860135976748325</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" si="2"/>
-        <v>76.476595391320416</v>
+        <v>74.399685488894193</v>
       </c>
       <c r="K12" s="3">
         <f t="shared" si="2"/>
-        <v>78.989910732819453</v>
+        <v>59.549625557516151</v>
       </c>
       <c r="L12" s="3">
         <f t="shared" si="2"/>
-        <v>69.593998132198294</v>
+        <v>55.363520224019794</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="2"/>
-        <v>43.281124831378747</v>
+        <v>57.182978635137147</v>
       </c>
       <c r="N12" s="3">
         <f t="shared" si="2"/>
-        <v>831.46104036750694</v>
+        <v>766.01472617069976</v>
       </c>
       <c r="O12" s="3">
         <f>O10-P4+O11</f>
-        <v>932.49965149694617</v>
+        <v>771.9879688667188</v>
       </c>
       <c r="Q12" s="3"/>
       <c r="S12" s="3"/>
     </row>
-    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="2">
         <f>B12/B10</f>
-        <v>4.0654000000000202E-3</v>
+        <v>2.2347567550614592E-3</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" ref="C13:O13" si="3">C12/C10</f>
-        <v>3.872800000000092E-3</v>
+        <v>3.7476100000000631E-3</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="3"/>
-        <v>3.8585599999999909E-3</v>
+        <v>3.844400000000016E-3</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="3"/>
-        <v>3.4590399999999107E-3</v>
+        <v>3.3337979999999621E-3</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="3"/>
-        <v>3.5553799999999232E-3</v>
+        <v>3.3337979999999152E-3</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="3"/>
-        <v>2.2066199999998836E-3</v>
+        <v>3.3337980000000167E-3</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="3"/>
-        <v>3.4590399999999033E-3</v>
+        <v>3.3337979999999057E-3</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="3"/>
-        <v>3.4590399999999211E-3</v>
+        <v>3.3337979999999707E-3</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="3"/>
-        <v>3.4590399999999107E-3</v>
+        <v>3.333798000000031E-3</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" si="3"/>
-        <v>3.4590399999999211E-3</v>
+        <v>2.6096270000000601E-3</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" si="3"/>
-        <v>3.1487199999999764E-3</v>
+        <v>2.5061739999999947E-3</v>
       </c>
       <c r="M13" s="2">
         <f t="shared" si="3"/>
-        <v>1.8959099999999863E-3</v>
+        <v>2.5061739999999652E-3</v>
       </c>
       <c r="N13" s="2">
         <f t="shared" si="3"/>
-        <v>3.3669651623434165E-3</v>
+        <v>3.1206896004176625E-3</v>
       </c>
       <c r="O13" s="2">
         <f t="shared" si="3"/>
-        <v>3.3561505372964404E-3</v>
+        <v>3.1268919999998751E-3</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="S13" s="2"/>
     </row>
-    <row r="14" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="71" t="s">
         <v>29</v>
       </c>
@@ -2338,7 +2461,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="72"/>
       <c r="B16" s="6" t="s">
         <v>5</v>
@@ -2378,7 +2501,7 @@
       </c>
       <c r="N16" s="74"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>0</v>
       </c>
@@ -2423,7 +2546,7 @@
         <v>267672.11300000001</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>1</v>
       </c>
@@ -2468,7 +2591,7 @@
         <v>96.337613040616304</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>2</v>
       </c>
@@ -2513,7 +2636,7 @@
         <v>71.458289083355865</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>3</v>
       </c>
@@ -2558,7 +2681,7 @@
         <v>40.240817019764272</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
         <v>4</v>
       </c>
@@ -2603,7 +2726,7 @@
         <v>-34.532430279868798</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="54"/>
       <c r="B22" s="54"/>
       <c r="C22" s="54"/>
@@ -2611,12 +2734,12 @@
       <c r="E22" s="54"/>
       <c r="F22" s="54"/>
     </row>
-    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="71" t="s">
         <v>31</v>
       </c>
@@ -2660,7 +2783,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="72"/>
       <c r="B25" s="6" t="s">
         <v>5</v>
@@ -2702,7 +2825,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>0</v>
       </c>
@@ -2747,7 +2870,7 @@
         <v>237900.00000000099</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>1</v>
       </c>
@@ -2792,7 +2915,7 @@
         <v>96.340235393022283</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>2</v>
       </c>
@@ -2837,7 +2960,7 @@
         <v>75.370529634300127</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>3</v>
       </c>
@@ -2882,7 +3005,7 @@
         <v>41.918411097099622</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
         <v>4</v>
       </c>
@@ -2972,9 +3095,9 @@
       <selection activeCell="N3" sqref="N3:N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="79" t="s">
         <v>32</v>
       </c>
@@ -3018,7 +3141,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="79"/>
       <c r="B2" s="28" t="s">
         <v>5</v>
@@ -3060,7 +3183,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -3104,7 +3227,7 @@
         <v>237900</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
@@ -3148,7 +3271,7 @@
         <v>96.340235393022283</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
@@ -3192,7 +3315,7 @@
         <v>76.583257671290454</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>3</v>
       </c>
@@ -3236,7 +3359,7 @@
         <v>42.307831021437579</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>4</v>
       </c>
@@ -3302,22 +3425,22 @@
       <selection pane="bottomRight" activeCell="B7" sqref="B7:M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="2" max="10" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="0.81640625" customWidth="1"/>
-    <col min="16" max="16" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="0.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="10" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="0.85546875" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="0.42578125" customWidth="1"/>
     <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="0.81640625" customWidth="1"/>
-    <col min="20" max="20" width="30.1796875" customWidth="1"/>
+    <col min="19" max="19" width="0.85546875" customWidth="1"/>
+    <col min="20" max="20" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="53"/>
       <c r="N1" s="4"/>
       <c r="O1" s="22">
@@ -3327,7 +3450,7 @@
       <c r="Q1" s="22"/>
       <c r="S1" s="22"/>
     </row>
-    <row r="2" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="86" t="s">
         <v>35</v>
       </c>
@@ -3380,7 +3503,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="86"/>
       <c r="B3" s="28" t="s">
         <v>5</v>
@@ -3427,56 +3550,56 @@
       <c r="R3" s="76"/>
       <c r="T3" s="78"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="26">
-        <f>[3]Produções!C88</f>
+        <f>[2]Produções!C88</f>
         <v>10705</v>
       </c>
       <c r="C4" s="26">
-        <f>[3]Produções!D88</f>
+        <f>[2]Produções!D88</f>
         <v>9616</v>
       </c>
       <c r="D4" s="26">
-        <f>[3]Produções!E88</f>
+        <f>[2]Produções!E88</f>
         <v>10705</v>
       </c>
       <c r="E4" s="26">
-        <f>[3]Produções!F88</f>
+        <f>[2]Produções!F88</f>
         <v>10342</v>
       </c>
       <c r="F4" s="26">
-        <f>[3]Produções!G88</f>
+        <f>[2]Produções!G88</f>
         <v>10705</v>
       </c>
       <c r="G4" s="26">
-        <f>[3]Produções!H88</f>
+        <f>[2]Produções!H88</f>
         <v>17237</v>
       </c>
       <c r="H4" s="26">
-        <f>[3]Produções!I88</f>
+        <f>[2]Produções!I88</f>
         <v>17842</v>
       </c>
       <c r="I4" s="26">
-        <f>[3]Produções!J88</f>
+        <f>[2]Produções!J88</f>
         <v>17842</v>
       </c>
       <c r="J4" s="26">
-        <f>[3]Produções!K88</f>
+        <f>[2]Produções!K88</f>
         <v>24132</v>
       </c>
       <c r="K4" s="26">
-        <f>[3]Produções!L88</f>
+        <f>[2]Produções!L88</f>
         <v>24978</v>
       </c>
       <c r="L4" s="26">
-        <f>[3]Produções!M88</f>
+        <f>[2]Produções!M88</f>
         <v>24132</v>
       </c>
       <c r="M4" s="26">
-        <f>[3]Produções!N88</f>
+        <f>[2]Produções!N88</f>
         <v>13064</v>
       </c>
       <c r="N4" s="49">
@@ -3484,7 +3607,7 @@
         <v>191300</v>
       </c>
       <c r="P4" s="42">
-        <f>[2]TL2!$N4</f>
+        <f>[3]TL2!$N4</f>
         <v>15010</v>
       </c>
       <c r="R4" s="36">
@@ -3493,7 +3616,7 @@
       </c>
       <c r="T4" s="29"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>1</v>
       </c>
@@ -3538,7 +3661,7 @@
         <v>95.317674856246725</v>
       </c>
       <c r="P5" s="41">
-        <f>[2]TL2!$N5</f>
+        <f>[3]TL2!$N5</f>
         <v>93.670886075949369</v>
       </c>
       <c r="R5" s="36">
@@ -3547,7 +3670,7 @@
       </c>
       <c r="T5" s="29"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>2</v>
       </c>
@@ -3592,7 +3715,7 @@
         <v>83.98414009409305</v>
       </c>
       <c r="P6" s="41">
-        <f>[2]TL2!$N6</f>
+        <f>[3]TL2!$N6</f>
         <v>100.00639819453697</v>
       </c>
       <c r="R6" s="36">
@@ -3601,7 +3724,7 @@
       </c>
       <c r="T6" s="29"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>3</v>
       </c>
@@ -3646,7 +3769,7 @@
         <v>43.774249869315213</v>
       </c>
       <c r="P7" s="41">
-        <f>[2]TL2!$N7</f>
+        <f>[3]TL2!$N7</f>
         <v>72.418387741505668</v>
       </c>
       <c r="R7" s="36">
@@ -3655,7 +3778,7 @@
       </c>
       <c r="T7" s="29"/>
     </row>
-    <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>4</v>
       </c>
@@ -3700,7 +3823,7 @@
         <v>-34.197769994772607</v>
       </c>
       <c r="P8" s="41">
-        <f>[2]TL2!$N8</f>
+        <f>[3]TL2!$N8</f>
         <v>-62.328447701532312</v>
       </c>
       <c r="R8" s="36">
@@ -3709,7 +3832,7 @@
       </c>
       <c r="T8" s="29"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="85"/>
       <c r="B9" s="85"/>
       <c r="C9" s="85"/>
@@ -3717,7 +3840,7 @@
       <c r="E9" s="85"/>
       <c r="F9" s="85"/>
     </row>
-    <row r="10" spans="1:20" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <f>B4/B5%</f>
         <v>11292.194092827005</v>
@@ -3781,7 +3904,7 @@
       <c r="Q10" s="3"/>
       <c r="S10" s="3"/>
     </row>
-    <row r="11" spans="1:20" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B8*B4/1000</f>
         <v>-418.56549999999999</v>
@@ -3845,7 +3968,7 @@
       <c r="Q11" s="3"/>
       <c r="S11" s="3"/>
     </row>
-    <row r="12" spans="1:20" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f>B10-B4+B11</f>
         <v>168.62859282700509</v>
@@ -3909,7 +4032,7 @@
       <c r="Q12" s="3"/>
       <c r="S12" s="3"/>
     </row>
-    <row r="13" spans="1:20" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3976,12 +4099,12 @@
       <c r="Q13" s="2"/>
       <c r="S13" s="2"/>
     </row>
-    <row r="15" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="71" t="s">
         <v>30</v>
       </c>
@@ -4032,7 +4155,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72"/>
       <c r="B17" s="6" t="s">
         <v>5</v>
@@ -4072,7 +4195,7 @@
       </c>
       <c r="N17" s="84"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>0</v>
       </c>
@@ -4117,7 +4240,7 @@
         <v>15010</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>1</v>
       </c>
@@ -4162,7 +4285,7 @@
         <v>93.670886075949369</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>2</v>
       </c>
@@ -4193,7 +4316,7 @@
         <v>100.00639819453697</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>3</v>
       </c>
@@ -4220,7 +4343,7 @@
         <v>72.418387741505668</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
         <v>4</v>
       </c>
@@ -4245,7 +4368,7 @@
         <v>-62.328447701532312</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="55"/>
       <c r="B23" s="55"/>
       <c r="C23" s="55"/>
@@ -4261,12 +4384,12 @@
       <c r="M23" s="56"/>
       <c r="N23" s="57"/>
     </row>
-    <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="71" t="s">
         <v>31</v>
       </c>
@@ -4310,7 +4433,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="72"/>
       <c r="B26" s="6" t="s">
         <v>5</v>
@@ -4352,7 +4475,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>0</v>
       </c>
@@ -4397,7 +4520,7 @@
         <v>191300</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>1</v>
       </c>
@@ -4442,7 +4565,7 @@
         <v>95.317674856246725</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>2</v>
       </c>
@@ -4487,7 +4610,7 @@
         <v>85.391364349189757</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>3</v>
       </c>
@@ -4532,7 +4655,7 @@
         <v>45.108082070047047</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="19" t="s">
         <v>4</v>
       </c>
@@ -4617,7 +4740,7 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -4631,12 +4754,12 @@
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="15" width="11.54296875" customWidth="1"/>
+    <col min="3" max="15" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C2" s="24" t="s">
         <v>33</v>
       </c>
@@ -4677,7 +4800,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C3" s="30" t="s">
         <v>5</v>
       </c>
@@ -4718,33 +4841,33 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="32">
         <f>'TL1'!B4</f>
-        <v>22000</v>
+        <v>17118.27</v>
       </c>
       <c r="D4" s="32">
         <f>'TL1'!C4</f>
-        <v>19900</v>
+        <v>20400</v>
       </c>
       <c r="E4" s="32">
         <f>'TL1'!D4</f>
-        <v>22000</v>
+        <v>23000</v>
       </c>
       <c r="F4" s="32">
         <f>'TL1'!E4</f>
-        <v>21300</v>
+        <v>21800</v>
       </c>
       <c r="G4" s="32">
         <f>'TL1'!F4</f>
-        <v>22000</v>
+        <v>22299.999999999003</v>
       </c>
       <c r="H4" s="32">
         <f>'TL1'!G4</f>
-        <v>10700</v>
+        <v>11200.000000000997</v>
       </c>
       <c r="I4" s="32">
         <f>'TL1'!H4</f>
@@ -4752,11 +4875,11 @@
       </c>
       <c r="J4" s="32">
         <f>'TL1'!I4</f>
-        <v>22000</v>
+        <v>22500</v>
       </c>
       <c r="K4" s="32">
         <f>'TL1'!J4</f>
-        <v>21300</v>
+        <v>21500</v>
       </c>
       <c r="L4" s="32">
         <f>'TL1'!K4</f>
@@ -4772,10 +4895,10 @@
       </c>
       <c r="O4" s="32">
         <f>SUM(C4:N4)</f>
-        <v>237900</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
+        <v>236518.27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="29" t="s">
         <v>19</v>
       </c>
@@ -4832,33 +4955,33 @@
         <v>191300</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="31" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="33">
         <f>SUM(C4:C5)</f>
-        <v>32705</v>
+        <v>27823.27</v>
       </c>
       <c r="D6" s="33">
         <f t="shared" ref="D6:O6" si="0">SUM(D4:D5)</f>
-        <v>29516</v>
+        <v>30016</v>
       </c>
       <c r="E6" s="33">
         <f t="shared" si="0"/>
-        <v>32705</v>
+        <v>33705</v>
       </c>
       <c r="F6" s="33">
         <f t="shared" si="0"/>
-        <v>31642</v>
+        <v>32142</v>
       </c>
       <c r="G6" s="33">
         <f t="shared" si="0"/>
-        <v>32705</v>
+        <v>33004.999999999003</v>
       </c>
       <c r="H6" s="33">
         <f t="shared" si="0"/>
-        <v>27937</v>
+        <v>28437.000000000997</v>
       </c>
       <c r="I6" s="33">
         <f t="shared" si="0"/>
@@ -4866,11 +4989,11 @@
       </c>
       <c r="J6" s="33">
         <f t="shared" si="0"/>
-        <v>39842</v>
+        <v>40342</v>
       </c>
       <c r="K6" s="33">
         <f t="shared" si="0"/>
-        <v>45432</v>
+        <v>45632</v>
       </c>
       <c r="L6" s="33">
         <f t="shared" si="0"/>
@@ -4886,15 +5009,15 @@
       </c>
       <c r="O6" s="33">
         <f t="shared" si="0"/>
-        <v>429200</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
+        <v>427818.27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" s="34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C10" s="28" t="s">
         <v>5</v>
       </c>
@@ -4935,7 +5058,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="29" t="s">
         <v>24</v>
       </c>
@@ -4992,30 +5115,30 @@
         <v>429200</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" s="4">
         <f>C6-C11</f>
-        <v>0</v>
+        <v>-4881.7299999999996</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" ref="D12:N12" si="1">D6-D11</f>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>299.99999999900319</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>500.00000000099681</v>
       </c>
       <c r="I12" s="4">
         <f t="shared" si="1"/>
@@ -5023,11 +5146,11 @@
       </c>
       <c r="J12" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="K12" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="L12" s="4">
         <f t="shared" si="1"/>
@@ -5043,7 +5166,7 @@
       </c>
       <c r="O12" s="4">
         <f>O6-O11</f>
-        <v>0</v>
+        <v>-1381.7299999999814</v>
       </c>
     </row>
   </sheetData>
@@ -5059,16 +5182,16 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7265625" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:17" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="4:17" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="62"/>
       <c r="E3" s="69" t="s">
         <v>5</v>
@@ -5110,7 +5233,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="4" spans="4:17" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="4:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D4" s="70" t="s">
         <v>0</v>
       </c>
@@ -5155,7 +5278,7 @@
         <v>237900</v>
       </c>
     </row>
-    <row r="5" spans="4:17" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="4:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D5" s="70" t="s">
         <v>45</v>
       </c>
@@ -5173,7 +5296,7 @@
       <c r="P5" s="64"/>
       <c r="Q5" s="64"/>
     </row>
-    <row r="6" spans="4:17" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="4:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D6" s="70" t="s">
         <v>1</v>
       </c>
@@ -5217,7 +5340,7 @@
         <v>96.336565783942831</v>
       </c>
     </row>
-    <row r="7" spans="4:17" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D7" s="70" t="s">
         <v>40</v>
       </c>
@@ -5262,7 +5385,7 @@
         <v>96.35564102564102</v>
       </c>
     </row>
-    <row r="8" spans="4:17" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="4:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D8" s="70" t="s">
         <v>2</v>
       </c>
@@ -5306,7 +5429,7 @@
         <v>75.278310214375793</v>
       </c>
     </row>
-    <row r="9" spans="4:17" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="4:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D9" s="70" t="s">
         <v>41</v>
       </c>
@@ -5351,7 +5474,7 @@
         <v>74.999579655317362</v>
       </c>
     </row>
-    <row r="10" spans="4:17" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="4:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D10" s="70" t="s">
         <v>3</v>
       </c>
@@ -5395,7 +5518,7 @@
         <v>41.865153425809162</v>
       </c>
     </row>
-    <row r="11" spans="4:17" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="4:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D11" s="70" t="s">
         <v>42</v>
       </c>
@@ -5440,7 +5563,7 @@
         <v>41.000336275746115</v>
       </c>
     </row>
-    <row r="12" spans="4:17" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="4:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D12" s="70" t="s">
         <v>39</v>
       </c>
@@ -5484,7 +5607,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="13" spans="4:17" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D13" s="70" t="s">
         <v>43</v>
       </c>
@@ -5529,7 +5652,7 @@
         <v>76.41</v>
       </c>
     </row>
-    <row r="14" spans="4:17" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="4:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D14" s="70" t="s">
         <v>44</v>
       </c>
@@ -5574,7 +5697,7 @@
         <v>76.2</v>
       </c>
     </row>
-    <row r="17" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P17" s="66"/>
     </row>
   </sheetData>
@@ -5595,6 +5718,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D9F4B9E5F21834EAD39AF5A901FB715" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eee3b99089d3c879cc490a9d6596ef41">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b4391c65-f8f3-4ea3-b99d-1bf2473f7170" xmlns:ns4="b1deae2b-0f26-434e-aee8-0827bfe3ac49" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d37873a4bed7158229cfef4f83f26dfb" ns3:_="" ns4:_="">
     <xsd:import namespace="b4391c65-f8f3-4ea3-b99d-1bf2473f7170"/>
@@ -5833,15 +5965,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2A430EF-9EED-4EDA-8CE9-FFCA665D44D8}">
   <ds:schemaRefs>
@@ -5860,6 +5983,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95F8991F-F93C-466C-9F57-E3AC92EECDEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B01EDC0C-59FA-46B4-A77F-263D2FE0B2F4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5876,12 +6007,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95F8991F-F93C-466C-9F57-E3AC92EECDEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>